<commit_message>
added results for the experiments
</commit_message>
<xml_diff>
--- a/Experiment_summary.xlsx
+++ b/Experiment_summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davitabrahamyan/Documents/UCSD/Projects/Fatemeh/human-eval-comm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davitabrahamyan/Documents/UCSD/Projects/Fatemeh/clarify-aware-coder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2309D84-2865-FE49-B392-258DA0207577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B346A815-FB0F-4649-B44F-59AE445A590E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{7FFB17F9-1DA1-8F4C-B591-3EC8B66B4365}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="37">
   <si>
     <t>Original</t>
   </si>
@@ -98,14 +98,62 @@
     <t>Current Status</t>
   </si>
   <si>
-    <t>Ongoing Evaluation</t>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Tokenizer</t>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>Codellama</t>
+  </si>
+  <si>
+    <t>Pass@1</t>
+  </si>
+  <si>
+    <t>Test Pass Rate</t>
+  </si>
+  <si>
+    <t>Comm Rate</t>
+  </si>
+  <si>
+    <t>Good Question Rate</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>Exp1</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>1p</t>
+  </si>
+  <si>
+    <t>2ac</t>
+  </si>
+  <si>
+    <t>2cp</t>
+  </si>
+  <si>
+    <t>2ap</t>
+  </si>
+  <si>
+    <t>3acp</t>
+  </si>
+  <si>
+    <t>Overall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,13 +167,87 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,13 +259,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -476,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDFC9BA-9932-B048-9939-A5E3EFC1DA9C}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,7 +636,7 @@
     <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -522,10 +665,13 @@
         <v>16</v>
       </c>
       <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -554,10 +700,13 @@
         <v>10</v>
       </c>
       <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -586,10 +735,13 @@
         <v>16</v>
       </c>
       <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -618,10 +770,13 @@
         <v>64</v>
       </c>
       <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -650,10 +805,13 @@
         <v>32</v>
       </c>
       <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -682,10 +840,13 @@
         <v>16</v>
       </c>
       <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -714,10 +875,13 @@
         <v>16</v>
       </c>
       <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -746,11 +910,1166 @@
         <v>64</v>
       </c>
       <c r="J8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>14.63</v>
+      </c>
+      <c r="D13" s="3">
+        <v>37.86</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3.66</v>
+      </c>
+      <c r="F13" s="3">
+        <v>21.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3">
+        <v>14.63</v>
+      </c>
+      <c r="D14" s="3">
+        <v>37.86</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3.66</v>
+      </c>
+      <c r="F14" s="3">
+        <v>25.61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="11">
+        <v>15.85</v>
+      </c>
+      <c r="D15" s="3">
+        <v>38.65</v>
+      </c>
+      <c r="E15" s="3">
+        <v>4.88</v>
+      </c>
+      <c r="F15" s="3">
+        <v>9.76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>15.24</v>
+      </c>
+      <c r="D16" s="11">
+        <v>39.770000000000003</v>
+      </c>
+      <c r="E16" s="3">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>14.02</v>
+      </c>
+      <c r="D17">
+        <v>38.340000000000003</v>
+      </c>
+      <c r="E17">
+        <v>0.61</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3">
+        <v>13.41</v>
+      </c>
+      <c r="D18" s="3">
+        <v>36.549999999999997</v>
+      </c>
+      <c r="E18" s="11">
+        <v>11.59</v>
+      </c>
+      <c r="F18" s="3">
+        <v>17.68</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3">
+        <v>14.63</v>
+      </c>
+      <c r="D19" s="3">
+        <v>37.409999999999997</v>
+      </c>
+      <c r="E19" s="3">
+        <v>6.71</v>
+      </c>
+      <c r="F19" s="11">
+        <v>36.590000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="3">
+        <v>13.41</v>
+      </c>
+      <c r="D20" s="3">
+        <v>38.35</v>
+      </c>
+      <c r="E20" s="3">
+        <v>3.05</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>32.520000000000003</v>
+      </c>
+      <c r="D22" s="3">
+        <v>51.05</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1.23</v>
+      </c>
+      <c r="F22" s="3">
+        <v>17.18</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="3">
+        <v>31.9</v>
+      </c>
+      <c r="D23" s="3">
+        <v>51.02</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="F23" s="3">
+        <v>16.559999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4">
+        <v>34.97</v>
+      </c>
+      <c r="D24" s="4">
+        <v>54.37</v>
+      </c>
+      <c r="E24">
+        <v>1.23</v>
+      </c>
+      <c r="F24">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3">
+        <v>33.130000000000003</v>
+      </c>
+      <c r="D25" s="3">
+        <v>53.71</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>31.29</v>
+      </c>
+      <c r="D26">
+        <v>51.9</v>
+      </c>
+      <c r="E26">
+        <v>1.23</v>
+      </c>
+      <c r="F26">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="3">
+        <v>31.29</v>
+      </c>
+      <c r="D27" s="3">
+        <v>51.67</v>
+      </c>
+      <c r="E27" s="12">
+        <v>5.52</v>
+      </c>
+      <c r="F27" s="3">
+        <v>7.36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3">
+        <v>33.74</v>
+      </c>
+      <c r="D28" s="3">
+        <v>51.47</v>
+      </c>
+      <c r="E28" s="3">
+        <v>5.52</v>
+      </c>
+      <c r="F28" s="12">
+        <v>27.61</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3">
+        <v>30.06</v>
+      </c>
+      <c r="D29" s="3">
+        <v>50.43</v>
+      </c>
+      <c r="E29" s="3">
+        <v>4.29</v>
+      </c>
+      <c r="F29" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3">
+        <v>9.76</v>
+      </c>
+      <c r="D31" s="3">
+        <v>27.97</v>
+      </c>
+      <c r="E31" s="3">
+        <v>6.71</v>
+      </c>
+      <c r="F31" s="3">
+        <v>19.510000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>9.15</v>
+      </c>
+      <c r="D32">
+        <v>29.19</v>
+      </c>
+      <c r="E32">
+        <v>0.61</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3">
+        <v>9.76</v>
+      </c>
+      <c r="D33" s="3">
+        <v>27.97</v>
+      </c>
+      <c r="E33" s="3">
+        <v>6.71</v>
+      </c>
+      <c r="F33" s="3">
+        <v>22.56</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="13">
+        <v>10.37</v>
+      </c>
+      <c r="D34" s="13">
+        <v>31.62</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1.22</v>
+      </c>
+      <c r="F34" s="3">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>7.32</v>
+      </c>
+      <c r="D35">
+        <v>27.2</v>
+      </c>
+      <c r="E35">
+        <v>5.49</v>
+      </c>
+      <c r="F35">
+        <v>14.02</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="3">
+        <v>4.88</v>
+      </c>
+      <c r="D36" s="3">
+        <v>22.71</v>
+      </c>
+      <c r="E36" s="13">
+        <v>23.17</v>
+      </c>
+      <c r="F36" s="3">
+        <v>20.12</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="3">
+        <v>9.15</v>
+      </c>
+      <c r="D37" s="3">
+        <v>26.51</v>
+      </c>
+      <c r="E37" s="3">
+        <v>11.59</v>
+      </c>
+      <c r="F37" s="13">
+        <v>38.409999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="D38" s="3">
+        <v>31.87</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1.83</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="19">
+        <v>14.81</v>
+      </c>
+      <c r="D40" s="14">
+        <v>35.92</v>
+      </c>
+      <c r="E40" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="F40" s="3">
+        <v>26.54</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41">
+        <v>12.35</v>
+      </c>
+      <c r="D41" s="6">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="E41">
+        <v>0.62</v>
+      </c>
+      <c r="F41">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="19">
+        <v>14.81</v>
+      </c>
+      <c r="D42" s="3">
+        <v>35.92</v>
+      </c>
+      <c r="E42" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="F42" s="3">
+        <v>25.93</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="3">
+        <v>11.73</v>
+      </c>
+      <c r="D43" s="3">
+        <v>35.81</v>
+      </c>
+      <c r="E43" s="3">
+        <v>3.09</v>
+      </c>
+      <c r="F43" s="3">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>8.64</v>
+      </c>
+      <c r="D44">
+        <v>34.75</v>
+      </c>
+      <c r="E44">
+        <v>4.32</v>
+      </c>
+      <c r="F44">
+        <v>11.11</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="3">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="D45" s="3">
+        <v>34.81</v>
+      </c>
+      <c r="E45" s="19">
+        <v>11.11</v>
+      </c>
+      <c r="F45" s="3">
+        <v>14.81</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="3">
+        <v>13.58</v>
+      </c>
+      <c r="D46" s="3">
+        <v>38</v>
+      </c>
+      <c r="E46" s="3">
+        <v>5.56</v>
+      </c>
+      <c r="F46" s="19">
+        <v>43.21</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="3">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="D47" s="3">
+        <v>33.619999999999997</v>
+      </c>
+      <c r="E47" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="F47" s="3">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="15">
+        <v>8.57</v>
+      </c>
+      <c r="D49" s="3">
+        <v>33.409999999999997</v>
+      </c>
+      <c r="E49" s="3">
+        <v>5.71</v>
+      </c>
+      <c r="F49" s="3">
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50">
+        <v>5.71</v>
+      </c>
+      <c r="D50">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>2.86</v>
+      </c>
+      <c r="D51">
+        <v>31.38</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="15">
+        <v>8.57</v>
+      </c>
+      <c r="D52" s="3">
+        <v>33.409999999999997</v>
+      </c>
+      <c r="E52" s="3">
+        <v>5.71</v>
+      </c>
+      <c r="F52" s="3">
+        <v>14.29</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="3">
+        <v>5.71</v>
+      </c>
+      <c r="D53" s="3">
+        <v>31.78</v>
+      </c>
+      <c r="E53" s="3">
+        <v>2.86</v>
+      </c>
+      <c r="F53" s="3">
+        <v>8.57</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="3">
+        <v>2.86</v>
+      </c>
+      <c r="D54" s="3">
+        <v>26.73</v>
+      </c>
+      <c r="E54" s="15">
+        <v>14.29</v>
+      </c>
+      <c r="F54" s="3">
+        <v>14.29</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="15">
+        <v>8.57</v>
+      </c>
+      <c r="D55" s="15">
+        <v>34.549999999999997</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+      <c r="F55" s="15">
+        <v>31.43</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="3">
+        <v>2.86</v>
+      </c>
+      <c r="D56" s="3">
+        <v>32</v>
+      </c>
+      <c r="E56" s="3">
+        <v>2.86</v>
+      </c>
+      <c r="F56" s="3">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B57" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="16">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="D58" s="3">
+        <v>22.35</v>
+      </c>
+      <c r="E58" s="3">
+        <v>15.49</v>
+      </c>
+      <c r="F58" s="3">
+        <v>32.39</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="3">
+        <v>5.63</v>
+      </c>
+      <c r="D59" s="16">
+        <v>23.89</v>
+      </c>
+      <c r="E59" s="3">
+        <v>2.86</v>
+      </c>
+      <c r="F59" s="3">
+        <v>4.2300000000000004</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>2.82</v>
+      </c>
+      <c r="D60">
+        <v>23.41</v>
+      </c>
+      <c r="E60">
+        <v>1.41</v>
+      </c>
+      <c r="F60">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="16">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="D61" s="3">
+        <v>22.35</v>
+      </c>
+      <c r="E61" s="3">
+        <v>15.49</v>
+      </c>
+      <c r="F61" s="3">
+        <v>30.99</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="3">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="D62" s="3">
+        <v>23.02</v>
+      </c>
+      <c r="E62" s="3">
+        <v>5.63</v>
+      </c>
+      <c r="F62" s="3">
+        <v>30.99</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="3">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="D63" s="3">
+        <v>14.28</v>
+      </c>
+      <c r="E63" s="16">
+        <v>39.44</v>
+      </c>
+      <c r="F63" s="3">
+        <v>38.03</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="3">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="D64" s="3">
+        <v>21.78</v>
+      </c>
+      <c r="E64" s="3">
+        <v>1.41</v>
+      </c>
+      <c r="F64" s="16">
+        <v>42.25</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="3">
+        <v>2.82</v>
+      </c>
+      <c r="D65" s="3">
+        <v>22.95</v>
+      </c>
+      <c r="E65" s="3">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B66" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="17">
+        <v>8.33</v>
+      </c>
+      <c r="D67" s="3">
+        <v>30.7</v>
+      </c>
+      <c r="E67" s="3">
+        <v>8.33</v>
+      </c>
+      <c r="F67" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" s="17">
+        <v>8.33</v>
+      </c>
+      <c r="D68" s="3">
+        <v>33.51</v>
+      </c>
+      <c r="E68" s="3">
+        <v>0</v>
+      </c>
+      <c r="F68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="9">
+        <v>8.33</v>
+      </c>
+      <c r="D69">
+        <v>33.51</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="17">
+        <v>8.33</v>
+      </c>
+      <c r="D70" s="3">
+        <v>30.7</v>
+      </c>
+      <c r="E70" s="3">
+        <v>8.33</v>
+      </c>
+      <c r="F70" s="3">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="17">
+        <v>8.33</v>
+      </c>
+      <c r="D71" s="3">
+        <v>31.43</v>
+      </c>
+      <c r="E71" s="3">
+        <v>0</v>
+      </c>
+      <c r="F71" s="3">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="17">
+        <v>8.33</v>
+      </c>
+      <c r="D72" s="3">
+        <v>26.57</v>
+      </c>
+      <c r="E72" s="17">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="F72" s="3">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="17">
+        <v>8.33</v>
+      </c>
+      <c r="D73" s="3">
+        <v>30.65</v>
+      </c>
+      <c r="E73" s="3">
+        <v>0</v>
+      </c>
+      <c r="F73" s="17">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" s="17">
+        <v>8.33</v>
+      </c>
+      <c r="D74" s="17">
+        <v>36.79</v>
+      </c>
+      <c r="E74" s="3">
+        <v>0</v>
+      </c>
+      <c r="F74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B75" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="3">
+        <v>14.66</v>
+      </c>
+      <c r="D76" s="3">
+        <v>37.270000000000003</v>
+      </c>
+      <c r="E76" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="F76" s="3">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>29</v>
+      </c>
+      <c r="C77" s="3">
+        <v>15.82</v>
+      </c>
+      <c r="D77" s="18">
+        <v>38.35</v>
+      </c>
+      <c r="E77" s="3">
+        <v>2.08</v>
+      </c>
+      <c r="F77" s="3">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="3">
+        <v>8.33</v>
+      </c>
+      <c r="D78" s="3">
+        <v>30.7</v>
+      </c>
+      <c r="E78" s="3">
+        <v>8.33</v>
+      </c>
+      <c r="F78" s="3">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="18">
+        <v>16.47</v>
+      </c>
+      <c r="D79" s="3">
+        <v>36.4</v>
+      </c>
+      <c r="E79" s="3">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="F79" s="3">
+        <v>21.66</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="3">
+        <v>14.92</v>
+      </c>
+      <c r="D80" s="3">
+        <v>36.85</v>
+      </c>
+      <c r="E80" s="3">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="F80" s="3">
+        <v>11.67</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="3">
+        <v>13.23</v>
+      </c>
+      <c r="D81" s="3">
+        <v>33.78</v>
+      </c>
+      <c r="E81" s="18">
+        <v>15.43</v>
+      </c>
+      <c r="F81" s="3">
+        <v>17.12</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="3">
+        <v>15.95</v>
+      </c>
+      <c r="D82" s="3">
+        <v>36.520000000000003</v>
+      </c>
+      <c r="E82" s="3">
+        <v>6.36</v>
+      </c>
+      <c r="F82" s="18">
+        <v>36.71</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" s="3">
+        <v>14.4</v>
+      </c>
+      <c r="D83" s="3">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="E83" s="3">
+        <v>2.85</v>
+      </c>
+      <c r="F83" s="3">
+        <v>1.69</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{2BEBE7E4-9E7F-0345-BEE7-31C23D783BF9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>